<commit_message>
Succesfully got board array printed
</commit_message>
<xml_diff>
--- a/Chess-engine/ArrayPlan.xlsx
+++ b/Chess-engine/ArrayPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingLanguages\INSANE-PROJECTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingLanguages\INSANE-PROJECTS\Chess-engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCEDFEAA-2847-4410-94B0-1CC154B6D333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE30B644-3326-44F7-AC38-69006E4EE6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{AA8A4C0C-8162-4E0A-B45E-7786839D6F73}"/>
   </bookViews>
@@ -200,14 +200,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:J15"/>
+      <selection activeCell="N4" sqref="N4:U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,15 +588,15 @@
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
     </row>
     <row r="2" spans="1:31" ht="25.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
@@ -639,15 +639,15 @@
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
     </row>
     <row r="3" spans="1:31" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -740,28 +740,28 @@
         <v>1</v>
       </c>
       <c r="N4" s="4">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="O4" s="5">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="P4" s="4">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="5">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="R4" s="4">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="S4" s="5">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="T4" s="4">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="U4" s="5">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -799,28 +799,28 @@
         <v>2</v>
       </c>
       <c r="N5" s="5">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="O5" s="4">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="P5" s="5">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="4">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="R5" s="5">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="S5" s="4">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="T5" s="5">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="U5" s="4">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -858,28 +858,28 @@
         <v>3</v>
       </c>
       <c r="N6" s="4">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="O6" s="5">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="P6" s="4">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="Q6" s="5">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="R6" s="4">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="S6" s="5">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="T6" s="4">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="U6" s="5">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -917,28 +917,28 @@
         <v>4</v>
       </c>
       <c r="N7" s="5">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="O7" s="4">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="P7" s="5">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="Q7" s="4">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="R7" s="5">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="S7" s="4">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="T7" s="5">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="U7" s="4">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -976,28 +976,28 @@
         <v>5</v>
       </c>
       <c r="N8" s="4">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="O8" s="5">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="P8" s="4">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="Q8" s="5">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="R8" s="4">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="S8" s="5">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="T8" s="4">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="U8" s="5">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1035,28 +1035,28 @@
         <v>6</v>
       </c>
       <c r="N9" s="5">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="O9" s="4">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="P9" s="5">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="Q9" s="4">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="R9" s="5">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="S9" s="4">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="T9" s="5">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="U9" s="4">
-        <v>78</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1094,28 +1094,28 @@
         <v>7</v>
       </c>
       <c r="N10" s="4">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="O10" s="5">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="P10" s="4">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="Q10" s="5">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="R10" s="4">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="S10" s="5">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="T10" s="4">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="U10" s="5">
-        <v>88</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1153,28 +1153,28 @@
         <v>8</v>
       </c>
       <c r="N11" s="5">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="O11" s="4">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="P11" s="5">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="Q11" s="4">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="R11" s="5">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="S11" s="4">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="T11" s="5">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="U11" s="4">
-        <v>98</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1208,24 +1208,24 @@
       <c r="J12" s="3">
         <v>119</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -1240,13 +1240,13 @@
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
@@ -1259,31 +1259,31 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
     </row>
     <row r="17" spans="15:21" x14ac:dyDescent="0.3">
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>